<commit_message>
working bottle, vial, vial with holes, using mcmaster spacer
</commit_message>
<xml_diff>
--- a/flyport_parameters.xlsx
+++ b/flyport_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinesh/Dropbox/Desktop_Sync/Inventor_Projects/custom_designs/fly_funnel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinesh/Dropbox/Desktop_Sync/Inventor_Projects/custom_designs/flyporter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0EC20B-D9CD-2346-9BE8-060E3CA91597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627A1517-067C-F745-97FA-1E16C97E13A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{B02287D1-4EF1-7A48-A112-9882D62F183C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>Parameter_Name</t>
   </si>
@@ -90,112 +90,160 @@
     <t>13 mm</t>
   </si>
   <si>
+    <t>0.1 mm</t>
+  </si>
+  <si>
+    <t>4 mm</t>
+  </si>
+  <si>
+    <t>top_D</t>
+  </si>
+  <si>
+    <t>cn_h</t>
+  </si>
+  <si>
+    <t>2 mm</t>
+  </si>
+  <si>
+    <t>w_th</t>
+  </si>
+  <si>
+    <t>w_l</t>
+  </si>
+  <si>
+    <t>wall thickness</t>
+  </si>
+  <si>
+    <t>wall length</t>
+  </si>
+  <si>
+    <t>outer diameter - larger vial</t>
+  </si>
+  <si>
+    <t>outer diameter - smaller vial - 12.25</t>
+  </si>
+  <si>
+    <t>t_D</t>
+  </si>
+  <si>
+    <t>tunnel diameter (M3/M4/M6)</t>
+  </si>
+  <si>
+    <t>top_th</t>
+  </si>
+  <si>
+    <t>top diameter</t>
+  </si>
+  <si>
+    <t>top thickness</t>
+  </si>
+  <si>
+    <t>connector height</t>
+  </si>
+  <si>
+    <t>lv_th</t>
+  </si>
+  <si>
+    <t>sv_th</t>
+  </si>
+  <si>
+    <t>t_D_f</t>
+  </si>
+  <si>
+    <t>tunnel diameter (female)</t>
+  </si>
+  <si>
+    <t>top thickness (female)</t>
+  </si>
+  <si>
+    <t>top_th_f</t>
+  </si>
+  <si>
+    <t>t_D + w_th</t>
+  </si>
+  <si>
+    <t>t_D_f + cn_h</t>
+  </si>
+  <si>
+    <t>10 mm</t>
+  </si>
+  <si>
+    <t>b_OD</t>
+  </si>
+  <si>
+    <t>b_th</t>
+  </si>
+  <si>
+    <t>outer diameter - bottle - 43.25</t>
+  </si>
+  <si>
+    <t>b_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inner diameter - bottle </t>
+  </si>
+  <si>
+    <t>b_rim_h</t>
+  </si>
+  <si>
+    <t>height of the bottle rim - 5.78</t>
+  </si>
+  <si>
+    <t>spacing between holes</t>
+  </si>
+  <si>
+    <t>h_s</t>
+  </si>
+  <si>
+    <t>h_D</t>
+  </si>
+  <si>
+    <t>hole diameter</t>
+  </si>
+  <si>
+    <t>cn_D</t>
+  </si>
+  <si>
+    <t>connector diameter (0.13 is mcmaster part 94669A014 tol)</t>
+  </si>
+  <si>
     <t>26 mm</t>
   </si>
   <si>
-    <t>0.1 mm</t>
-  </si>
-  <si>
-    <t>4 mm</t>
-  </si>
-  <si>
-    <t>top_D</t>
-  </si>
-  <si>
-    <t>cn_h</t>
-  </si>
-  <si>
-    <t>2 mm</t>
-  </si>
-  <si>
-    <t>w_th</t>
-  </si>
-  <si>
-    <t>w_l</t>
-  </si>
-  <si>
-    <t>wall thickness</t>
-  </si>
-  <si>
-    <t>wall length</t>
-  </si>
-  <si>
-    <t>outer diameter - larger vial</t>
-  </si>
-  <si>
-    <t>outer diameter - smaller vial - 12.25</t>
-  </si>
-  <si>
-    <t>t_D</t>
-  </si>
-  <si>
-    <t>tunnel diameter (M3/M4/M6)</t>
-  </si>
-  <si>
-    <t>top_th</t>
-  </si>
-  <si>
-    <t>top diameter</t>
-  </si>
-  <si>
-    <t>top thickness</t>
-  </si>
-  <si>
-    <t>connector height</t>
-  </si>
-  <si>
-    <t>lv_th</t>
-  </si>
-  <si>
-    <t>sv_th</t>
-  </si>
-  <si>
-    <t>t_D_f</t>
-  </si>
-  <si>
-    <t>tunnel diameter (female)</t>
-  </si>
-  <si>
-    <t>top thickness (female)</t>
-  </si>
-  <si>
-    <t>top_th_f</t>
-  </si>
-  <si>
-    <t>t_D + w_th</t>
-  </si>
-  <si>
-    <t>t_D_f + cn_h</t>
-  </si>
-  <si>
-    <t>10 mm</t>
-  </si>
-  <si>
-    <t>b_OD</t>
-  </si>
-  <si>
-    <t>b_th</t>
-  </si>
-  <si>
-    <t>43.5 mm</t>
-  </si>
-  <si>
-    <t>outer diameter - bottle - 43.25</t>
-  </si>
-  <si>
-    <t>b_ID</t>
-  </si>
-  <si>
-    <t>37 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inner diameter - bottle </t>
-  </si>
-  <si>
-    <t>b_rim_h</t>
-  </si>
-  <si>
-    <t>height of the bottle rim - 5.78</t>
+    <t>36.5 mm</t>
+  </si>
+  <si>
+    <t>v_h_D</t>
+  </si>
+  <si>
+    <t>vial hole diameter</t>
+  </si>
+  <si>
+    <t>7.5 mm</t>
+  </si>
+  <si>
+    <t>v_h_off</t>
+  </si>
+  <si>
+    <t>offset distance of hole center from the vial center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cn_D/2 + v_h_D/2 </t>
+  </si>
+  <si>
+    <t>6 mm + 1*tol</t>
+  </si>
+  <si>
+    <t>44 mm</t>
+  </si>
+  <si>
+    <t>0.75 mm</t>
+  </si>
+  <si>
+    <t>1.6 mm</t>
+  </si>
+  <si>
+    <t>2.5 mm</t>
   </si>
 </sst>
 </file>
@@ -547,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DE42A4-FACF-A24D-B8A4-F427B1EB0157}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +627,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -593,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -604,7 +652,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -613,12 +661,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -627,203 +675,273 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried M5 and M6 combinations, made holed versions of vial, bottle M6
</commit_message>
<xml_diff>
--- a/flyport_parameters.xlsx
+++ b/flyport_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinesh/Dropbox/Desktop_Sync/Inventor_Projects/custom_designs/flyporter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627A1517-067C-F745-97FA-1E16C97E13A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E3230E-C82B-7543-B558-4D91924EDBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{B02287D1-4EF1-7A48-A112-9882D62F183C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Parameter_Name</t>
   </si>
@@ -93,9 +93,6 @@
     <t>0.1 mm</t>
   </si>
   <si>
-    <t>4 mm</t>
-  </si>
-  <si>
     <t>top_D</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t xml:space="preserve">cn_D/2 + v_h_D/2 </t>
   </si>
   <si>
-    <t>6 mm + 1*tol</t>
-  </si>
-  <si>
     <t>44 mm</t>
   </si>
   <si>
@@ -243,7 +237,10 @@
     <t>1.6 mm</t>
   </si>
   <si>
-    <t>2.5 mm</t>
+    <t>13 mm + 1.5*tol</t>
+  </si>
+  <si>
+    <t>2.25 mm</t>
   </si>
 </sst>
 </file>
@@ -598,7 +595,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -652,7 +649,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -661,12 +658,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -675,96 +672,96 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -773,7 +770,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -781,21 +778,21 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -815,12 +812,12 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -834,21 +831,21 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -862,21 +859,21 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -885,63 +882,63 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>59</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working models M6 bottle, vial & parameters
</commit_message>
<xml_diff>
--- a/flyport_parameters.xlsx
+++ b/flyport_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinesh/Dropbox/Desktop_Sync/Inventor_Projects/custom_designs/flyporter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E3230E-C82B-7543-B558-4D91924EDBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57874D4E-BCEC-0D41-B7D9-3346FC8E84D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{B02287D1-4EF1-7A48-A112-9882D62F183C}"/>
   </bookViews>
@@ -237,10 +237,10 @@
     <t>1.6 mm</t>
   </si>
   <si>
-    <t>13 mm + 1.5*tol</t>
-  </si>
-  <si>
     <t>2.25 mm</t>
+  </si>
+  <si>
+    <t>13 mm + 2*tol</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -904,7 +904,7 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
increased hole diameter and number; works well
</commit_message>
<xml_diff>
--- a/flyport_parameters.xlsx
+++ b/flyport_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinesh/Dropbox/Desktop_Sync/Inventor_Projects/custom_designs/flyporter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57874D4E-BCEC-0D41-B7D9-3346FC8E84D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230469EB-7093-0E4E-A769-F89C121AE74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{B02287D1-4EF1-7A48-A112-9882D62F183C}"/>
   </bookViews>
@@ -231,9 +231,6 @@
     <t>44 mm</t>
   </si>
   <si>
-    <t>0.75 mm</t>
-  </si>
-  <si>
     <t>1.6 mm</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>13 mm + 2*tol</t>
+  </si>
+  <si>
+    <t>0.90 mm</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -792,7 +792,7 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -890,7 +890,7 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -904,7 +904,7 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>